<commit_message>
Version 2.0.1 solucionado error espera de base de datos
</commit_message>
<xml_diff>
--- a/reportes/10.10.11.150.xlsx
+++ b/reportes/10.10.11.150.xlsx
@@ -31,10 +31,10 @@
     <t>No. Expediente Clínico</t>
   </si>
   <si>
-    <t xml:space="preserve">      </t>
-  </si>
-  <si>
-    <t>/201758431</t>
+    <t xml:space="preserve">11111111111  22222222222    </t>
+  </si>
+  <si>
+    <t>/201761854</t>
   </si>
   <si>
     <t>Fecha de Nacimiento ( Dia Mes Año)</t>
@@ -49,13 +49,13 @@
     <t>Sexo M  (   )   F  (    )</t>
   </si>
   <si>
-    <t>2017-10-05</t>
+    <t>2017-10-04</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>77</t>
+    <t>2112</t>
   </si>
   <si>
     <t>MASCULINO</t>
@@ -88,13 +88,13 @@
     <t>Fecha de la asistencia Médica</t>
   </si>
   <si>
-    <t>Hora: 15:44:45</t>
+    <t>Hora: 10:41:45</t>
   </si>
   <si>
     <t>Area de urgencia: null</t>
   </si>
   <si>
-    <t>19/10/2017</t>
+    <t>23/10/2017</t>
   </si>
   <si>
     <t>MEDICINA</t>

</xml_diff>